<commit_message>
Update Pertanggal 9 Januari 2026 20:00 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/SysConfig.TblMapper_LDAPUserToPerson.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/SysConfig.TblMapper_LDAPUserToPerson.xlsx
@@ -19078,10 +19078,10 @@
   <dimension ref="B1:K631"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C593" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H604" sqref="H604"/>
+      <selection pane="bottomRight" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -19930,11 +19930,11 @@
         <v>Fikri</v>
       </c>
       <c r="E30" s="34">
-        <v>25000000000154</v>
+        <v>25000000000155</v>
       </c>
       <c r="F30" s="30" t="str">
         <f>IF(EXACT($E30, ""), "", VLOOKUP($E30, [2]DataLookUp!$B$4:$C$618, 2, FALSE))</f>
-        <v>Fikri</v>
+        <v>M. Fikri Caesarandi Hasibuan</v>
       </c>
       <c r="H30" s="20">
         <f t="shared" si="0"/>
@@ -19942,7 +19942,7 @@
       </c>
       <c r="I30" s="19" t="str">
         <f t="shared" si="1"/>
-        <v>PERFORM "SchSysConfig"."Func_TblMapper_LDAPUserToPerson_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 47000000000027::bigint, 25000000000154::bigint);</v>
+        <v>PERFORM "SchSysConfig"."Func_TblMapper_LDAPUserToPerson_SET"(varSystemLoginSession, null::bigint, null::varchar, null::timestamptz, null::timestamptz, null::varchar, varInstitutionBranchID, varBaseCurrencyID, 47000000000027::bigint, 25000000000155::bigint);</v>
       </c>
       <c r="K30" s="34"/>
     </row>

</xml_diff>